<commit_message>
update groundwater, working upload
</commit_message>
<xml_diff>
--- a/data/dov_template.xlsx
+++ b/data/dov_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Realdolmen\DOV\PFAS_Antwerpen\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vlaamseoverheid-my.sharepoint.com/personal/guillaume_vandekerckhove_vlaanderen_be/Documents/Documenten/PycharmProjects/xls2xml/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CC9D60-8516-4DAC-A125-C9FCAC8EDA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{5B856FD6-B847-4BDA-B540-A8FC34361A93}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{5B856FD6-B847-4BDA-B540-A8FC34361A93}"/>
   </bookViews>
   <sheets>
     <sheet name="bodemlocaties" sheetId="1" r:id="rId1"/>
@@ -510,7 +510,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -526,7 +526,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2520,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94A994C-364A-4A44-8577-1FAE296E37A2}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2637,7 +2637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00656A7A-C711-487E-8A5C-68E6F6141D3B}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>